<commit_message>
Added main norming ANOVAS
In tables_figures script, and in results_section script, all the
norming anovas are complete, with all relevant comparisons.
</commit_message>
<xml_diff>
--- a/Tables_Figures/output/table02_SR_relatedness_ratings.xlsx
+++ b/Tables_Figures/output/table02_SR_relatedness_ratings.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Local.Noun.Number</t>
   </si>
@@ -21,9 +21,6 @@
   </si>
   <si>
     <t>Unrelated</t>
-  </si>
-  <si>
-    <t>pval</t>
   </si>
   <si>
     <t>1</t>
@@ -72,9 +69,6 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
-  </si>
-  <si>
-    <t>7.97772e-13 ***</t>
   </si>
 </sst>
 </file>
@@ -136,76 +130,61 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>